<commit_message>
statement web - ver - 1.1
</commit_message>
<xml_diff>
--- a/04_pandas/statements/statement_7k.xlsx
+++ b/04_pandas/statements/statement_7k.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="159">
   <si>
     <t xml:space="preserve">Ticket</t>
   </si>
@@ -470,6 +470,33 @@
   </si>
   <si>
     <t xml:space="preserve">2021.09.15 13:35:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 11:48:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 13:35:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 06:50:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 21:07:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 06:56:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 07:24:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 08:52:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 09:20:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021.09.16 13:45:09</t>
   </si>
 </sst>
 </file>
@@ -570,13 +597,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K90" activeCellId="0" sqref="K90"/>
+      <selection pane="topLeft" activeCell="P114" activeCellId="0" sqref="P114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5592,6 +5619,314 @@
       </c>
       <c r="N114" s="0" t="n">
         <v>81.82</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>109125567</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>15453.67</v>
+      </c>
+      <c r="G115" s="0" t="n">
+        <v>15453.35</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <v>15511</v>
+      </c>
+      <c r="I115" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="J115" s="0" t="n">
+        <v>15453.35</v>
+      </c>
+      <c r="K115" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N115" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>109122880</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>15487.69</v>
+      </c>
+      <c r="G116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J116" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K116" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N116" s="0" t="n">
+        <v>37.76</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>109122889</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>15485.67</v>
+      </c>
+      <c r="G117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J117" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K117" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N117" s="0" t="n">
+        <v>40.9</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>109122983</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>15481.06</v>
+      </c>
+      <c r="G118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J118" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K118" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" s="0" t="n">
+        <v>48.06</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>109123618</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>15473.06</v>
+      </c>
+      <c r="G119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J119" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K119" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" s="0" t="n">
+        <v>60.48</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>109124227</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>15495.31</v>
+      </c>
+      <c r="G120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J120" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K120" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N120" s="0" t="n">
+        <v>25.92</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>109126351</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>15454.06</v>
+      </c>
+      <c r="G121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J121" s="0" t="n">
+        <v>15512</v>
+      </c>
+      <c r="K121" s="0" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="L121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N121" s="0" t="n">
+        <v>89.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>